<commit_message>
fix the fix (fixing M11+14 introduced a bug in "create new user" dialog)
</commit_message>
<xml_diff>
--- a/documents/time-records/Wagner_Claudia_csaw9017.xlsx
+++ b/documents/time-records/Wagner_Claudia_csaw9017.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\miDev\uni\git.uibk\informatik\qe\sepsss21\group1\g1t1\time-records\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\miDev\uni\git.uibk\informatik\qe\sepsss21\group1\g1t1\documents\time-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997AD273-D46A-4425-A43C-F134A87DE0D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF11D964-8320-488B-AE67-06E5ECE1763B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="50">
   <si>
     <t>Datum</t>
   </si>
@@ -161,13 +161,50 @@
   <si>
     <t>Use Case User Editieren durch Admin</t>
   </si>
+  <si>
+    <t>User Case Game Erstellen</t>
+  </si>
+  <si>
+    <t>User Case Teams Erstellen</t>
+  </si>
+  <si>
+    <t>Game- and Team-related Tests</t>
+  </si>
+  <si>
+    <t>Use Case Term/Topic-Upload</t>
+  </si>
+  <si>
+    <t>Term- and Topic-related Tests</t>
+  </si>
+  <si>
+    <t>Feature Einheitliche VirtualLobby</t>
+  </si>
+  <si>
+    <t>Use Case Spielereinladung</t>
+  </si>
+  <si>
+    <t>Erweiterung/Verbesserung bestehender Funktionalitäten</t>
+  </si>
+  <si>
+    <t>Feature Anwesenheitscheck im Gameroom</t>
+  </si>
+  <si>
+    <t>Feature Echtzeitupdate</t>
+  </si>
+  <si>
+    <t>Datenbanktrennung und Fixes</t>
+  </si>
+  <si>
+    <t>Bugfixes Abnahmetest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -240,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -255,6 +292,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -569,24 +607,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:D1018"/>
+  <dimension ref="A1:E1018"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D49" sqref="D49"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="9.625" customWidth="1"/>
-    <col min="3" max="3" width="37.375" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="55.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="31.5">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="31.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -600,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="8">
         <v>44256</v>
       </c>
@@ -613,8 +651,9 @@
       <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="8">
         <v>44256</v>
       </c>
@@ -628,7 +667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="8">
         <v>44261</v>
       </c>
@@ -642,7 +681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="8">
         <v>44263</v>
       </c>
@@ -656,7 +695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="8">
         <v>44263</v>
       </c>
@@ -670,7 +709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="8">
         <v>44264</v>
       </c>
@@ -684,7 +723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="8">
         <v>44264</v>
       </c>
@@ -698,7 +737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="8">
         <v>44265</v>
       </c>
@@ -712,7 +751,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="8">
         <v>44265</v>
       </c>
@@ -726,7 +765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="8">
         <v>44268</v>
       </c>
@@ -740,7 +779,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="8">
         <v>44269</v>
       </c>
@@ -754,7 +793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="8">
         <v>44269</v>
       </c>
@@ -768,7 +807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="8">
         <v>44271</v>
       </c>
@@ -782,7 +821,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="8">
         <v>44277</v>
       </c>
@@ -796,7 +835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="8">
         <v>44278</v>
       </c>
@@ -1245,169 +1284,466 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="8"/>
-      <c r="B48" s="7"/>
-      <c r="D48" s="3"/>
+      <c r="A48" s="8">
+        <v>44310</v>
+      </c>
+      <c r="B48" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="8"/>
-      <c r="B49" s="7"/>
-      <c r="D49" s="3"/>
+      <c r="A49" s="8">
+        <v>44311</v>
+      </c>
+      <c r="B49" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="8"/>
-      <c r="B50" s="7"/>
-      <c r="D50" s="3"/>
+      <c r="A50" s="8">
+        <v>44311</v>
+      </c>
+      <c r="B50" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="8"/>
-      <c r="B51" s="7"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="8">
+        <v>44312</v>
+      </c>
+      <c r="B51" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="8"/>
-      <c r="B52" s="7"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="8">
+        <v>44313</v>
+      </c>
+      <c r="B52" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="8"/>
-      <c r="B53" s="7"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="8">
+        <v>44313</v>
+      </c>
+      <c r="B53" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="8"/>
-      <c r="B54" s="7"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="8">
+        <v>44315</v>
+      </c>
+      <c r="B54" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="7"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="8">
+        <v>44316</v>
+      </c>
+      <c r="B55" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="8"/>
-      <c r="B56" s="7"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="8">
+        <v>44317</v>
+      </c>
+      <c r="B56" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="8"/>
-      <c r="B57" s="7"/>
-      <c r="D57" s="3"/>
+      <c r="A57" s="8">
+        <v>44317</v>
+      </c>
+      <c r="B57" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="8"/>
-      <c r="B58" s="7"/>
-      <c r="D58" s="3"/>
+      <c r="A58" s="8">
+        <v>44318</v>
+      </c>
+      <c r="B58" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="8"/>
-      <c r="B59" s="7"/>
-      <c r="D59" s="3"/>
+      <c r="A59" s="8">
+        <v>44318</v>
+      </c>
+      <c r="B59" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="8"/>
-      <c r="B60" s="7"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="8">
+        <v>44320</v>
+      </c>
+      <c r="B60" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="8"/>
-      <c r="B61" s="7"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="8">
+        <v>44320</v>
+      </c>
+      <c r="B61" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="8"/>
-      <c r="B62" s="7"/>
-      <c r="D62" s="3"/>
+      <c r="A62" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B62" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="8"/>
-      <c r="B63" s="7"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="8">
+        <v>44323</v>
+      </c>
+      <c r="B63" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="8"/>
-      <c r="B64" s="7"/>
-      <c r="D64" s="3"/>
+      <c r="A64" s="8">
+        <v>44324</v>
+      </c>
+      <c r="B64" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="8"/>
-      <c r="B65" s="7"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="8">
+        <v>44324</v>
+      </c>
+      <c r="B65" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="8"/>
-      <c r="B66" s="7"/>
-      <c r="D66" s="3"/>
+      <c r="A66" s="8">
+        <v>44325</v>
+      </c>
+      <c r="B66" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="8"/>
-      <c r="B67" s="7"/>
-      <c r="D67" s="3"/>
+      <c r="A67" s="8">
+        <v>44325</v>
+      </c>
+      <c r="B67" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="8"/>
-      <c r="B68" s="7"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B68" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="8"/>
-      <c r="B69" s="7"/>
-      <c r="D69" s="3"/>
+      <c r="A69" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B69" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="8"/>
-      <c r="B70" s="7"/>
-      <c r="D70" s="3"/>
+      <c r="A70" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B70" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="8"/>
-      <c r="B71" s="7"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B71" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="8"/>
-      <c r="B72" s="7"/>
-      <c r="D72" s="3"/>
+      <c r="A72" s="8">
+        <v>44328</v>
+      </c>
+      <c r="B72" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="8"/>
-      <c r="B73" s="7"/>
-      <c r="D73" s="3"/>
+      <c r="A73" s="8">
+        <v>44329</v>
+      </c>
+      <c r="B73" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="8"/>
-      <c r="B74" s="7"/>
-      <c r="D74" s="3"/>
+      <c r="A74" s="8">
+        <v>44329</v>
+      </c>
+      <c r="B74" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="8"/>
-      <c r="B75" s="7"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="8">
+        <v>44333</v>
+      </c>
+      <c r="B75" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="8"/>
-      <c r="B76" s="7"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="8">
+        <v>44334</v>
+      </c>
+      <c r="B76" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="8"/>
-      <c r="B77" s="7"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="8">
+        <v>44335</v>
+      </c>
+      <c r="B77" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="8"/>
-      <c r="B78" s="7"/>
-      <c r="D78" s="3"/>
+      <c r="A78" s="8">
+        <v>44336</v>
+      </c>
+      <c r="B78" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="8"/>
-      <c r="B79" s="7"/>
-      <c r="D79" s="3"/>
+      <c r="A79" s="8">
+        <v>44343</v>
+      </c>
+      <c r="B79" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="8"/>
-      <c r="B80" s="7"/>
-      <c r="D80" s="3"/>
+      <c r="A80" s="8">
+        <v>44343</v>
+      </c>
+      <c r="B80" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="8"/>

</xml_diff>

<commit_message>
remove unused skeleton remains
</commit_message>
<xml_diff>
--- a/documents/time-records/Wagner_Claudia_csaw9017.xlsx
+++ b/documents/time-records/Wagner_Claudia_csaw9017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\miDev\uni\git.uibk\informatik\qe\sepsss21\group1\g1t1\documents\time-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967068C4-EBF2-454E-8440-E137C8D05006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63182FD1-6E29-4884-94B2-7FDD881279DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="17550" windowHeight="14910" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="60">
   <si>
     <t>Datum</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Feature Spiel von aussen anhalten, abbrechen</t>
+  </si>
+  <si>
+    <t>Bugfixes und optionale Features</t>
+  </si>
+  <si>
+    <t>Cleanup und Durchtesten</t>
   </si>
 </sst>
 </file>
@@ -634,10 +640,10 @@
   <dimension ref="A1:F1018"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2023,14 +2029,32 @@
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="8"/>
-      <c r="B99" s="7"/>
-      <c r="D99" s="3"/>
+      <c r="A99" s="8">
+        <v>44359</v>
+      </c>
+      <c r="B99" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="8"/>
-      <c r="B100" s="7"/>
-      <c r="D100" s="3"/>
+      <c r="A100" s="8">
+        <v>44360</v>
+      </c>
+      <c r="B100" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="8"/>

</xml_diff>

<commit_message>
- add javadoc pluging to pom - complete and correct javadoc comments
</commit_message>
<xml_diff>
--- a/documents/time-records/Wagner_Claudia_csaw9017.xlsx
+++ b/documents/time-records/Wagner_Claudia_csaw9017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\miDev\uni\git.uibk\informatik\qe\sepsss21\group1\g1t1\documents\time-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63182FD1-6E29-4884-94B2-7FDD881279DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5712EF31-CA77-4324-83C7-3EED40F04185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="17550" windowHeight="14910" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -225,7 +225,7 @@
     <t>Bugfixes und optionale Features</t>
   </si>
   <si>
-    <t>Cleanup und Durchtesten</t>
+    <t>Cleanup, Durchtesten, Javadoc-Generierung</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A1:F1018"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B101" sqref="B101"/>
@@ -2047,7 +2047,7 @@
         <v>44360</v>
       </c>
       <c r="B100" s="7">
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
- add check for players in multiple teams when creating game - fix game cancel/halt/revive
</commit_message>
<xml_diff>
--- a/documents/time-records/Wagner_Claudia_csaw9017.xlsx
+++ b/documents/time-records/Wagner_Claudia_csaw9017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\miDev\uni\git.uibk\informatik\qe\sepsss21\group1\g1t1\documents\time-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5712EF31-CA77-4324-83C7-3EED40F04185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556F0BA5-DC3D-4265-BF77-9E93185087CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="17550" windowHeight="14910" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="62">
   <si>
     <t>Datum</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Cleanup, Durchtesten, Javadoc-Generierung</t>
+  </si>
+  <si>
+    <t>Javadoc-Generierung, Bugfix Game Abbrechen</t>
+  </si>
+  <si>
+    <t>Bugfix Game Anhalten</t>
   </si>
 </sst>
 </file>
@@ -640,10 +646,10 @@
   <dimension ref="A1:F1018"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B101" sqref="B101"/>
+      <selection pane="bottomRight" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2057,24 +2063,60 @@
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="8"/>
-      <c r="B101" s="7"/>
-      <c r="D101" s="3"/>
+      <c r="A101" s="8">
+        <v>44360</v>
+      </c>
+      <c r="B101" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="8"/>
-      <c r="B102" s="7"/>
-      <c r="D102" s="3"/>
+      <c r="A102" s="8">
+        <v>44361</v>
+      </c>
+      <c r="B102" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="8"/>
-      <c r="B103" s="7"/>
-      <c r="D103" s="3"/>
+      <c r="A103" s="8">
+        <v>44362</v>
+      </c>
+      <c r="B103" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="8"/>
-      <c r="B104" s="7"/>
-      <c r="D104" s="3"/>
+      <c r="A104" s="8">
+        <v>44363</v>
+      </c>
+      <c r="B104" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="8"/>

</xml_diff>